<commit_message>
style changes for insert order and admin side
</commit_message>
<xml_diff>
--- a/misc/ETC.xlsx
+++ b/misc/ETC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOWORK\Desktop\XAMPP\htdocs\temp_folder\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480BAE2E-FAA1-45F3-91DC-0E83BF1730D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5F25C5-BA00-4337-AF8F-7DB13D990CAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>GO:WORK</t>
   </si>
@@ -201,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,15 +224,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,11 +235,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -321,12 +309,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -344,13 +331,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -365,23 +349,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,21 +654,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="3"/>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -792,10 +771,10 @@
       <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="16"/>
+      <c r="M9" s="15"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
@@ -890,10 +869,10 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="1"/>
       <c r="L17" s="4">
         <v>43741</v>
@@ -1023,10 +1002,10 @@
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="16"/>
+      <c r="D27" s="15"/>
       <c r="L27" s="4">
         <v>43759</v>
       </c>
@@ -1113,10 +1092,10 @@
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="G34" s="18" t="s">
+      <c r="G34" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="19"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
@@ -1146,7 +1125,7 @@
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="16" t="s">
         <v>41</v>
       </c>
       <c r="D38">
@@ -1156,27 +1135,27 @@
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="17"/>
-      <c r="G39" s="14" t="s">
+      <c r="C39" s="16"/>
+      <c r="G39" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="15"/>
+      <c r="H39" s="21"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H40" s="21"/>
+      <c r="H40" s="14"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="16"/>
-      <c r="G41" s="20" t="s">
+      <c r="D41" s="15"/>
+      <c r="G41" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="H41" s="21"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
@@ -1185,10 +1164,10 @@
       <c r="D42" s="5">
         <v>0.33</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="G42" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H42" s="21"/>
+      <c r="H42" s="14"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
@@ -1197,10 +1176,10 @@
       <c r="D43" s="5">
         <v>0.33</v>
       </c>
-      <c r="G43" s="24" t="s">
+      <c r="G43" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H43" s="24"/>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="5" t="s">
@@ -1209,10 +1188,10 @@
       <c r="D44" s="5">
         <v>0.5</v>
       </c>
-      <c r="G44" s="22" t="s">
+      <c r="G44" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H44" s="23"/>
+      <c r="H44" s="14"/>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
@@ -1239,10 +1218,10 @@
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H47" s="15"/>
+      <c r="H47" s="21"/>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
@@ -1288,7 +1267,7 @@
       <c r="H52" s="7"/>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G53" s="13" t="s">
+      <c r="G53" s="19" t="s">
         <v>41</v>
       </c>
       <c r="H53" s="7">
@@ -1296,7 +1275,7 @@
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G54" s="13"/>
+      <c r="G54" s="19"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
@@ -1304,10 +1283,10 @@
       <c r="H55" s="7"/>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G56" s="14" t="s">
+      <c r="G56" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H56" s="15"/>
+      <c r="H56" s="21"/>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G57" s="6" t="s">
@@ -1347,6 +1326,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C41:D41"/>
@@ -1354,12 +1339,6 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed multiple kladder bug
</commit_message>
<xml_diff>
--- a/misc/ETC.xlsx
+++ b/misc/ETC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOWORK\Desktop\XAMPP\htdocs\temp_folder\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5F25C5-BA00-4337-AF8F-7DB13D990CAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77B0619-21AD-4AE9-A0CA-0AEADEB4A367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -337,6 +337,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -349,15 +358,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -642,7 +644,7 @@
   <dimension ref="C3:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,21 +656,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="18"/>
       <c r="I3" s="3"/>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -771,10 +773,10 @@
       <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="15"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
@@ -869,10 +871,10 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="1"/>
       <c r="L17" s="4">
         <v>43741</v>
@@ -1002,10 +1004,10 @@
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="15"/>
+      <c r="D27" s="18"/>
       <c r="L27" s="4">
         <v>43759</v>
       </c>
@@ -1092,10 +1094,10 @@
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="G34" s="17" t="s">
+      <c r="G34" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="18"/>
+      <c r="H34" s="21"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
@@ -1117,15 +1119,15 @@
       <c r="C37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G37" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="23">
         <v>2.5</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="19" t="s">
         <v>41</v>
       </c>
       <c r="D38">
@@ -1135,11 +1137,11 @@
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="16"/>
-      <c r="G39" s="20" t="s">
+      <c r="C39" s="19"/>
+      <c r="G39" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="21"/>
+      <c r="H39" s="17"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G40" s="13" t="s">
@@ -1148,10 +1150,10 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="15"/>
+      <c r="D41" s="18"/>
       <c r="G41" s="13" t="s">
         <v>48</v>
       </c>
@@ -1218,10 +1220,10 @@
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G47" s="20" t="s">
+      <c r="G47" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H47" s="21"/>
+      <c r="H47" s="17"/>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
@@ -1267,7 +1269,7 @@
       <c r="H52" s="7"/>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G53" s="19" t="s">
+      <c r="G53" s="15" t="s">
         <v>41</v>
       </c>
       <c r="H53" s="7">
@@ -1275,7 +1277,7 @@
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G54" s="19"/>
+      <c r="G54" s="15"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
@@ -1283,10 +1285,10 @@
       <c r="H55" s="7"/>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G56" s="20" t="s">
+      <c r="G56" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H56" s="21"/>
+      <c r="H56" s="17"/>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G57" s="6" t="s">
@@ -1326,12 +1328,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C41:D41"/>
@@ -1339,6 +1335,12 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added preview upload functionality
</commit_message>
<xml_diff>
--- a/misc/ETC.xlsx
+++ b/misc/ETC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOWORK\Desktop\XAMPP\htdocs\temp_folder\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77B0619-21AD-4AE9-A0CA-0AEADEB4A367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A399F6-06B7-4AF7-9BAA-EC1445026303}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>GO:WORK</t>
   </si>
@@ -195,13 +195,16 @@
   </si>
   <si>
     <t>Edit Kladde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix search fields </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,8 +227,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +245,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -309,11 +324,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -337,15 +353,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -358,11 +369,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -641,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:N61"/>
+  <dimension ref="C3:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,21 +675,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="18"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="18"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="3"/>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -773,10 +792,10 @@
       <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="18"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
@@ -871,10 +890,10 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="1"/>
       <c r="L17" s="4">
         <v>43741</v>
@@ -1004,10 +1023,10 @@
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="18"/>
+      <c r="D27" s="19"/>
       <c r="L27" s="4">
         <v>43759</v>
       </c>
@@ -1094,10 +1113,10 @@
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G34" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="21"/>
+      <c r="H34" s="22"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
@@ -1119,15 +1138,15 @@
       <c r="C37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H37" s="23">
+      <c r="H37" s="16">
         <v>2.5</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="20" t="s">
         <v>41</v>
       </c>
       <c r="D38">
@@ -1137,11 +1156,11 @@
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="19"/>
-      <c r="G39" s="16" t="s">
+      <c r="C39" s="20"/>
+      <c r="G39" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="17"/>
+      <c r="H39" s="25"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G40" s="13" t="s">
@@ -1150,10 +1169,10 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="18"/>
+      <c r="D41" s="19"/>
       <c r="G41" s="13" t="s">
         <v>48</v>
       </c>
@@ -1202,10 +1221,10 @@
       <c r="D45" s="5">
         <v>0.5</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G45" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="H45" s="7">
+      <c r="H45" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1220,10 +1239,10 @@
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G47" s="16" t="s">
+      <c r="G47" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="H47" s="17"/>
+      <c r="H47" s="25"/>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
@@ -1241,7 +1260,7 @@
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G49" s="6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H49" s="7"/>
     </row>
@@ -1254,80 +1273,92 @@
         <v>69.66</v>
       </c>
       <c r="G50" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G51" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H50" s="7"/>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G51" s="6"/>
       <c r="H51" s="7"/>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="6"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G53" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G53" s="15" t="s">
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G54" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H53" s="7">
+      <c r="H54" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G54" s="15"/>
-      <c r="H54" s="7"/>
-    </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G55" s="6"/>
+      <c r="G55" s="23"/>
       <c r="H55" s="7"/>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G56" s="16" t="s">
+      <c r="G56" s="6"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G57" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H56" s="17"/>
-    </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G57" s="6" t="s">
+      <c r="H57" s="25"/>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G58" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H57" s="7">
+      <c r="H58" s="7">
         <v>1.5</v>
-      </c>
-    </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G58" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H58" s="7">
-        <v>2.5</v>
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G59" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H59" s="7">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G60" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H60" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G61" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G61" s="11" t="s">
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G62" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H61" s="12"/>
+      <c r="H62" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C41:D41"/>
@@ -1335,12 +1366,6 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed csv export and mark as complete
</commit_message>
<xml_diff>
--- a/misc/ETC.xlsx
+++ b/misc/ETC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOWORK\Desktop\XAMPP\htdocs\temp_folder\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A399F6-06B7-4AF7-9BAA-EC1445026303}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90208F87-8E11-4699-A998-7C801DE4B6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>GO:WORK</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t xml:space="preserve">Fix search fields </t>
+  </si>
+  <si>
+    <t xml:space="preserve">on completed orders/ kladder, aktive?, </t>
+  </si>
+  <si>
+    <t>Backup databasen- Find hosting som tilbyder backup. Siteground, Hostinger, Blue Host</t>
   </si>
 </sst>
 </file>
@@ -357,6 +363,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,14 +381,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -663,7 +669,7 @@
   <dimension ref="C3:N62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,21 +681,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="19"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="3"/>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -792,10 +798,10 @@
       <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="19"/>
+      <c r="M9" s="21"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
@@ -890,10 +896,10 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="1"/>
       <c r="L17" s="4">
         <v>43741</v>
@@ -1023,10 +1029,10 @@
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="19"/>
+      <c r="D27" s="21"/>
       <c r="L27" s="4">
         <v>43759</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="5" t="s">
         <v>18</v>
       </c>
@@ -1106,19 +1112,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="G34" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="22"/>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="24"/>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
         <v>33</v>
       </c>
@@ -1128,13 +1134,13 @@
       <c r="G35" s="6"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G36" s="8" t="s">
         <v>42</v>
       </c>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
         <v>40</v>
       </c>
@@ -1145,8 +1151,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="s">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
         <v>41</v>
       </c>
       <c r="D38">
@@ -1155,30 +1161,30 @@
       <c r="G38" s="6"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="20"/>
-      <c r="G39" s="24" t="s">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="22"/>
+      <c r="G39" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="25"/>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="20"/>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G40" s="13" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="14"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="19" t="s">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="19"/>
+      <c r="D41" s="21"/>
       <c r="G41" s="13" t="s">
         <v>48</v>
       </c>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1196,7 @@
       </c>
       <c r="H42" s="14"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
         <v>5</v>
       </c>
@@ -1202,7 +1208,7 @@
       </c>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="5" t="s">
         <v>6</v>
       </c>
@@ -1214,21 +1220,21 @@
       </c>
       <c r="H44" s="14"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D45" s="5">
         <v>0.5</v>
       </c>
-      <c r="G45" s="17" t="s">
+      <c r="G45" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H45" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>20</v>
       </c>
@@ -1238,31 +1244,34 @@
       <c r="G46" s="6"/>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G47" s="24" t="s">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G47" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H47" s="25"/>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="20"/>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D48">
         <v>5</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="G48" s="17" t="s">
         <v>46</v>
       </c>
       <c r="H48" s="7">
         <v>4.5</v>
       </c>
+      <c r="I48" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G49" s="6" t="s">
+      <c r="G49" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H49" s="7"/>
+      <c r="H49" s="16"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
@@ -1272,16 +1281,16 @@
         <f>SUM(D1:D49)</f>
         <v>69.66</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="G50" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="H50" s="7"/>
+      <c r="H50" s="18"/>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G51" s="6" t="s">
+      <c r="G51" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="H51" s="7"/>
+      <c r="H51" s="18"/>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G52" s="6"/>
@@ -1294,15 +1303,15 @@
       <c r="H53" s="7"/>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G54" s="23" t="s">
-        <v>41</v>
+      <c r="G54" s="25" t="s">
+        <v>56</v>
       </c>
       <c r="H54" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G55" s="23"/>
+      <c r="G55" s="25"/>
       <c r="H55" s="7"/>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
@@ -1310,10 +1319,10 @@
       <c r="H56" s="7"/>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G57" s="24" t="s">
+      <c r="G57" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H57" s="25"/>
+      <c r="H57" s="20"/>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G58" s="6" t="s">
@@ -1353,12 +1362,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C41:D41"/>
@@ -1366,6 +1369,12 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed live mails from kladder and gowork side
</commit_message>
<xml_diff>
--- a/misc/ETC.xlsx
+++ b/misc/ETC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22307"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOWORK\Desktop\XAMPP\htdocs\temp_folder\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90208F87-8E11-4699-A998-7C801DE4B6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2564116D-18EA-401E-A7AE-279230692AE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>GO:WORK</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Backup databasen- Find hosting som tilbyder backup. Siteground, Hostinger, Blue Host</t>
+  </si>
+  <si>
+    <t>Send confirmation mail (kladder og insert)</t>
+  </si>
+  <si>
+    <t>en mail adresse til hver</t>
   </si>
 </sst>
 </file>
@@ -335,7 +341,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -363,12 +369,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -384,6 +384,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -666,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:N62"/>
+  <dimension ref="C3:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,21 +689,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="3"/>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -798,10 +806,10 @@
       <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="21"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
@@ -896,10 +904,10 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="1"/>
       <c r="L17" s="4">
         <v>43741</v>
@@ -1029,10 +1037,10 @@
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="21"/>
+      <c r="D27" s="19"/>
       <c r="L27" s="4">
         <v>43759</v>
       </c>
@@ -1103,28 +1111,40 @@
       <c r="D32" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L32" s="4">
+        <v>43781</v>
+      </c>
+      <c r="M32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D33" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="L33" s="4">
+        <v>43782</v>
+      </c>
+      <c r="M33">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="G34" s="23" t="s">
+      <c r="G34" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="24"/>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
         <v>33</v>
       </c>
@@ -1134,13 +1154,13 @@
       <c r="G35" s="6"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G36" s="8" t="s">
         <v>42</v>
       </c>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
         <v>40</v>
       </c>
@@ -1151,8 +1171,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="22" t="s">
+    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C38" s="20" t="s">
         <v>41</v>
       </c>
       <c r="D38">
@@ -1161,30 +1181,30 @@
       <c r="G38" s="6"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="22"/>
-      <c r="G39" s="19" t="s">
+    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C39" s="20"/>
+      <c r="G39" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="20"/>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H39" s="25"/>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G40" s="13" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="14"/>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="21" t="s">
+    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C41" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="21"/>
+      <c r="D41" s="19"/>
       <c r="G41" s="13" t="s">
         <v>48</v>
       </c>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
         <v>4</v>
       </c>
@@ -1196,84 +1216,87 @@
       </c>
       <c r="H42" s="14"/>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="5">
         <v>0.33</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G43" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C44" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="5">
         <v>0.5</v>
       </c>
-      <c r="G44" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H44" s="14"/>
-    </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G44" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H44" s="5"/>
+      <c r="I44" s="26"/>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D45" s="5">
         <v>0.5</v>
       </c>
-      <c r="G45" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H45" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G45" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H45" s="14"/>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>20</v>
       </c>
       <c r="D46">
         <v>2</v>
       </c>
-      <c r="G46" s="6"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G47" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="H47" s="20"/>
-    </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G46" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G47" s="6"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D48">
         <v>5</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="G48" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H48" s="25"/>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G49" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H49" s="7">
         <v>4.5</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G49" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H49" s="16"/>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
         <v>32</v>
       </c>
@@ -1281,87 +1304,99 @@
         <f>SUM(D1:D49)</f>
         <v>69.66</v>
       </c>
-      <c r="G50" s="17" t="s">
+      <c r="G50" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G51" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="H50" s="18"/>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G51" s="17" t="s">
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="H51" s="18"/>
-    </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G52" s="6"/>
-      <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G53" s="8" t="s">
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="6"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H53" s="7"/>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G54" s="25" t="s">
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="H54" s="7">
+      <c r="H55" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G55" s="25"/>
-      <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G56" s="6"/>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="23"/>
       <c r="H56" s="7"/>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G57" s="19" t="s">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G57" s="6"/>
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G58" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H57" s="20"/>
-    </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G58" s="6" t="s">
+      <c r="H58" s="25"/>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G59" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H58" s="7">
+      <c r="H59" s="7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G59" s="10" t="s">
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H60" s="7">
         <v>2.5</v>
       </c>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G60" s="10" t="s">
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G61" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H60" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="G61" s="10" t="s">
+      <c r="H61" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G62" s="11" t="s">
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G63" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H62" s="12"/>
+      <c r="H63" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C41:D41"/>
@@ -1369,12 +1404,6 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed login landing page and navbar
</commit_message>
<xml_diff>
--- a/misc/ETC.xlsx
+++ b/misc/ETC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOWORK\Desktop\XAMPP\htdocs\temp_folder\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2564116D-18EA-401E-A7AE-279230692AE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC4362F-26AE-497A-99C5-907414F8EF4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="64">
   <si>
     <t>GO:WORK</t>
   </si>
@@ -210,13 +210,28 @@
   </si>
   <si>
     <t>en mail adresse til hver</t>
+  </si>
+  <si>
+    <t>Delete Kladder</t>
+  </si>
+  <si>
+    <t>Mark aktive as complete on login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header footer in log in </t>
+  </si>
+  <si>
+    <t>User per Fakultet ansvar</t>
+  </si>
+  <si>
+    <t>Fix Header Menu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +257,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -341,7 +362,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -369,6 +390,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -381,17 +413,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -674,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:N63"/>
+  <dimension ref="C3:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,21 +712,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="19"/>
+      <c r="H3" s="24"/>
       <c r="I3" s="3"/>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -806,10 +829,10 @@
       <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="19"/>
+      <c r="M9" s="24"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
@@ -904,10 +927,10 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="1"/>
       <c r="L17" s="4">
         <v>43741</v>
@@ -1037,10 +1060,10 @@
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="19"/>
+      <c r="D27" s="24"/>
       <c r="L27" s="4">
         <v>43759</v>
       </c>
@@ -1139,10 +1162,10 @@
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="G34" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="22"/>
+      <c r="H34" s="27"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
@@ -1172,7 +1195,7 @@
       </c>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="25" t="s">
         <v>41</v>
       </c>
       <c r="D38">
@@ -1182,11 +1205,11 @@
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C39" s="20"/>
-      <c r="G39" s="24" t="s">
+      <c r="C39" s="25"/>
+      <c r="G39" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="25"/>
+      <c r="H39" s="23"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G40" s="13" t="s">
@@ -1195,10 +1218,10 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="19"/>
+      <c r="D41" s="24"/>
       <c r="G41" s="13" t="s">
         <v>48</v>
       </c>
@@ -1223,9 +1246,10 @@
       <c r="D43" s="5">
         <v>0.33</v>
       </c>
-      <c r="G43" s="27" t="s">
+      <c r="G43" s="5" t="s">
         <v>57</v>
       </c>
+      <c r="H43" s="5"/>
       <c r="I43" s="2" t="s">
         <v>58</v>
       </c>
@@ -1241,7 +1265,7 @@
         <v>53</v>
       </c>
       <c r="H44" s="5"/>
-      <c r="I44" s="26"/>
+      <c r="I44" s="19"/>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
@@ -1250,10 +1274,10 @@
       <c r="D45" s="5">
         <v>0.5</v>
       </c>
-      <c r="G45" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H45" s="14"/>
+      <c r="G45" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H45" s="5"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
@@ -1262,16 +1286,16 @@
       <c r="D46">
         <v>2</v>
       </c>
-      <c r="G46" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H46" s="16">
-        <v>1</v>
-      </c>
+      <c r="G46" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" s="20"/>
     </row>
     <row r="47" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G47" s="6"/>
-      <c r="H47" s="7"/>
+      <c r="G47" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H47" s="28"/>
     </row>
     <row r="48" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
@@ -1280,21 +1304,16 @@
       <c r="D48">
         <v>5</v>
       </c>
-      <c r="G48" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="H48" s="25"/>
+      <c r="G48" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" s="28"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G49" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="H49" s="7">
-        <v>4.5</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="G49" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H49" s="5"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
@@ -1304,99 +1323,128 @@
         <f>SUM(D1:D49)</f>
         <v>69.66</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="G50" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G51" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H51" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="6"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53" s="23"/>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H54" s="16">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H50" s="16"/>
-    </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G51" s="17" t="s">
+      <c r="H55" s="16"/>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="H51" s="18"/>
-    </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G52" s="17" t="s">
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G57" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="H52" s="18"/>
-    </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G53" s="6"/>
-      <c r="H53" s="7"/>
-    </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G54" s="8" t="s">
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G58" s="6"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G59" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G55" s="23" t="s">
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="H55" s="7">
+      <c r="H60" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G56" s="23"/>
-      <c r="H56" s="7"/>
-    </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G57" s="6"/>
-      <c r="H57" s="7"/>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G58" s="24" t="s">
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G61" s="21"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="6"/>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G63" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H58" s="25"/>
-    </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G59" s="6" t="s">
+      <c r="H63" s="23"/>
+    </row>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G64" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H64" s="7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G60" s="10" t="s">
+    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G65" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H60" s="7">
+      <c r="H65" s="7">
         <v>2.5</v>
       </c>
     </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G61" s="10" t="s">
+    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G66" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H61" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G62" s="10" t="s">
+      <c r="H66" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G67" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G63" s="11" t="s">
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G68" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H63" s="12"/>
+      <c r="H68" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C41:D41"/>
@@ -1404,6 +1452,12 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added specific fakultet on all pages
</commit_message>
<xml_diff>
--- a/misc/ETC.xlsx
+++ b/misc/ETC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOWORK\Desktop\XAMPP\htdocs\temp_folder\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC4362F-26AE-497A-99C5-907414F8EF4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640B9F2-BBC0-41DC-BF3E-5251C657CBD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
   <si>
     <t>GO:WORK</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>Fix Header Menu</t>
+  </si>
+  <si>
+    <t>User per Fakultet skal opdateres I kladder og completed</t>
+  </si>
+  <si>
+    <t>Bestilt den: plus timestamp</t>
   </si>
 </sst>
 </file>
@@ -286,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -356,13 +362,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -391,16 +412,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,8 +424,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -697,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:N68"/>
+  <dimension ref="C3:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="M58" sqref="M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,21 +734,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="24"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="24"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="3"/>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -829,10 +851,10 @@
       <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="24"/>
+      <c r="M9" s="20"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
@@ -927,10 +949,10 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="1"/>
       <c r="L17" s="4">
         <v>43741</v>
@@ -1060,10 +1082,10 @@
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="24"/>
+      <c r="D27" s="20"/>
       <c r="L27" s="4">
         <v>43759</v>
       </c>
@@ -1162,10 +1184,10 @@
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="G34" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="27"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
@@ -1195,7 +1217,7 @@
       </c>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="21" t="s">
         <v>41</v>
       </c>
       <c r="D38">
@@ -1205,11 +1227,11 @@
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C39" s="25"/>
-      <c r="G39" s="22" t="s">
+      <c r="C39" s="21"/>
+      <c r="G39" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="23"/>
+      <c r="H39" s="26"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G40" s="13" t="s">
@@ -1218,10 +1240,10 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="24"/>
+      <c r="D41" s="20"/>
       <c r="G41" s="13" t="s">
         <v>48</v>
       </c>
@@ -1286,16 +1308,16 @@
       <c r="D46">
         <v>2</v>
       </c>
-      <c r="G46" s="20" t="s">
+      <c r="G46" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H46" s="20"/>
+      <c r="H46" s="5"/>
     </row>
     <row r="47" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G47" s="29" t="s">
+      <c r="G47" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H47" s="28"/>
+      <c r="H47" s="30"/>
     </row>
     <row r="48" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
@@ -1304,16 +1326,16 @@
       <c r="D48">
         <v>5</v>
       </c>
-      <c r="G48" s="29" t="s">
+      <c r="G48" s="27" t="s">
         <v>62</v>
       </c>
       <c r="H48" s="28"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G49" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H49" s="5"/>
+      <c r="G49" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="28"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
@@ -1323,128 +1345,146 @@
         <f>SUM(D1:D49)</f>
         <v>69.66</v>
       </c>
-      <c r="G50" s="13" t="s">
+      <c r="G50" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H50" s="28"/>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G51" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H50" s="14"/>
-    </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G51" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H51" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G52" s="6"/>
-      <c r="H52" s="7"/>
+      <c r="H52" s="14"/>
       <c r="I52" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G53" s="22" t="s">
+      <c r="G53" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H53" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="6"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H53" s="23"/>
-    </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G54" s="15" t="s">
+      <c r="H55" s="26"/>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H54" s="16">
+      <c r="H56" s="16">
         <v>4.5</v>
       </c>
     </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G55" s="15" t="s">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G57" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H55" s="16"/>
-    </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G56" s="17" t="s">
+      <c r="H57" s="16"/>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G58" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="H56" s="18"/>
-    </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G57" s="17" t="s">
+      <c r="H58" s="18"/>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G59" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H57" s="18"/>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G58" s="6"/>
-      <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G59" s="8" t="s">
+      <c r="H59" s="16"/>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="6"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G61" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G60" s="21" t="s">
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H60" s="7">
+      <c r="H62" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G61" s="21"/>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G62" s="6"/>
-      <c r="H62" s="7"/>
-    </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G63" s="22" t="s">
+      <c r="G63" s="24"/>
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G64" s="6"/>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G65" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H63" s="23"/>
-    </row>
-    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G64" s="6" t="s">
+      <c r="H65" s="26"/>
+    </row>
+    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G66" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H64" s="7">
+      <c r="H66" s="7">
         <v>1.5</v>
-      </c>
-    </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G65" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H65" s="7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G66" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H66" s="7">
-        <v>2</v>
       </c>
     </row>
     <row r="67" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G67" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" s="7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="68" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G68" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H68" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G69" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H67" s="7"/>
-    </row>
-    <row r="68" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G68" s="11" t="s">
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G70" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H68" s="12"/>
+      <c r="H70" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C41:D41"/>
@@ -1452,12 +1492,6 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added order_send_date on client side
</commit_message>
<xml_diff>
--- a/misc/ETC.xlsx
+++ b/misc/ETC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOWORK\Desktop\XAMPP\htdocs\temp_folder\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F640B9F2-BBC0-41DC-BF3E-5251C657CBD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EA50DC-250A-463A-A889-9BC9B5C22490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>GO:WORK</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Bestilt den: plus timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bekræftelsesmail? </t>
   </si>
 </sst>
 </file>
@@ -409,9 +412,20 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,19 +438,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -719,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:N70"/>
+  <dimension ref="C3:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,21 +737,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="20"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="20"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="3"/>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -851,10 +854,10 @@
       <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="L9" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="20"/>
+      <c r="M9" s="25"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
@@ -949,10 +952,10 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="1"/>
       <c r="L17" s="4">
         <v>43741</v>
@@ -1082,10 +1085,10 @@
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="20"/>
+      <c r="D27" s="25"/>
       <c r="L27" s="4">
         <v>43759</v>
       </c>
@@ -1184,10 +1187,10 @@
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="23"/>
+      <c r="H34" s="28"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
@@ -1217,7 +1220,7 @@
       </c>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="26" t="s">
         <v>41</v>
       </c>
       <c r="D38">
@@ -1227,11 +1230,11 @@
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C39" s="21"/>
-      <c r="G39" s="25" t="s">
+      <c r="C39" s="26"/>
+      <c r="G39" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="26"/>
+      <c r="H39" s="24"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G40" s="13" t="s">
@@ -1240,10 +1243,10 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="20"/>
+      <c r="D41" s="25"/>
       <c r="G41" s="13" t="s">
         <v>48</v>
       </c>
@@ -1287,7 +1290,7 @@
         <v>53</v>
       </c>
       <c r="H44" s="5"/>
-      <c r="I44" s="19"/>
+      <c r="I44" s="17"/>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
@@ -1314,10 +1317,10 @@
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G47" s="30" t="s">
+      <c r="G47" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="H47" s="30"/>
+      <c r="H47" s="21"/>
     </row>
     <row r="48" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
@@ -1326,16 +1329,16 @@
       <c r="D48">
         <v>5</v>
       </c>
-      <c r="G48" s="27" t="s">
+      <c r="G48" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="H48" s="28"/>
+      <c r="H48" s="19"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G49" s="29" t="s">
+      <c r="G49" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="H49" s="28"/>
+      <c r="H49" s="19"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
@@ -1345,146 +1348,146 @@
         <f>SUM(D1:D49)</f>
         <v>69.66</v>
       </c>
-      <c r="G50" s="29" t="s">
+      <c r="G50" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="H50" s="28"/>
+      <c r="H50" s="19"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G51" s="5" t="s">
+      <c r="G51" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="H51" s="30"/>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G52" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H52" s="14"/>
+      <c r="H52" s="5"/>
       <c r="I52" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G53" s="15" t="s">
+      <c r="G53" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H53" s="14"/>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H53" s="16">
+      <c r="H54" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G54" s="6"/>
-      <c r="H54" s="7"/>
-    </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G55" s="25" t="s">
+      <c r="G55" s="6"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H55" s="26"/>
-    </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G56" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H56" s="16">
-        <v>4.5</v>
-      </c>
+      <c r="H56" s="24"/>
     </row>
     <row r="57" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G57" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H57" s="16">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G58" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H57" s="16"/>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G58" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H58" s="18"/>
+      <c r="H58" s="16"/>
     </row>
     <row r="59" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G59" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H59" s="16"/>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H59" s="16"/>
-    </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G60" s="6"/>
-      <c r="H60" s="7"/>
+      <c r="H60" s="16"/>
     </row>
     <row r="61" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G61" s="8" t="s">
+      <c r="G61" s="6"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G62" s="24" t="s">
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G63" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="H62" s="7">
+      <c r="H63" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G63" s="24"/>
-      <c r="H63" s="7"/>
-    </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G64" s="6"/>
+      <c r="G64" s="22"/>
       <c r="H64" s="7"/>
     </row>
     <row r="65" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G65" s="25" t="s">
+      <c r="G65" s="6"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G66" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H65" s="26"/>
-    </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G66" s="6" t="s">
+      <c r="H66" s="24"/>
+    </row>
+    <row r="67" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G67" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H66" s="7">
+      <c r="H67" s="7">
         <v>1.5</v>
-      </c>
-    </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G67" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H67" s="7">
-        <v>2.5</v>
       </c>
     </row>
     <row r="68" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G68" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H68" s="7">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="69" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G69" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H69" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G70" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G70" s="11" t="s">
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G71" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H70" s="12"/>
+      <c r="H71" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C41:D41"/>
@@ -1492,6 +1495,12 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>